<commit_message>
Upload of data after editor comments
</commit_message>
<xml_diff>
--- a/data_folder/biofilm data.xlsx
+++ b/data_folder/biofilm data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/aoe_sniprbiome_com/Documents/projects/SNIPR001 paper/data/new_data_folder/experimental_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/aoe_sniprbiome_com/Documents/projects/SNIPR001 paper/paper_resub_clean/data_folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{F0F57584-9FD9-8A48-99CB-6035DD8B608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF14FD0-D566-EA41-A9B9-EE1943F6DC82}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{F0F57584-9FD9-8A48-99CB-6035DD8B608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C13112A0-A401-3B4A-B2E7-A6BFED797065}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F8053CE2-95FE-B34C-A11E-2EFB61C6A076}"/>
+    <workbookView xWindow="28800" yWindow="-1800" windowWidth="28800" windowHeight="18000" xr2:uid="{F8053CE2-95FE-B34C-A11E-2EFB61C6A076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,10 +46,10 @@
     <t>repeat</t>
   </si>
   <si>
-    <t>Promoter A</t>
+    <t>P_bolA</t>
   </si>
   <si>
-    <t>Promoter B</t>
+    <t>P_relB</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,10 +440,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>

</xml_diff>